<commit_message>
Fixed Home Scroll too
</commit_message>
<xml_diff>
--- a/public/documents/iAqua Aquatics Transship List.xlsx
+++ b/public/documents/iAqua Aquatics Transship List.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harutyun/Library/Messages/Attachments/c6/06/06F5EC31-BFC7-453A-AAAD-2ACE4BDF662B/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harutyun/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECECA9B-129C-FE47-8D75-E42DF7CD959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C11651A-2F40-CA4B-815F-857AA55CA5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Transship" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -63,6 +62,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -73,6 +73,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -83,6 +84,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -96,6 +98,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -106,6 +109,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -116,6 +120,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -129,6 +134,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -142,6 +148,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -152,6 +159,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -162,6 +170,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -175,6 +184,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -185,6 +195,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -195,6 +206,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -208,6 +220,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -218,6 +231,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -228,6 +242,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -241,6 +256,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -254,6 +270,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -264,6 +281,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -274,6 +292,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -353,6 +372,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -366,6 +386,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -379,6 +400,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -392,6 +414,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -405,6 +428,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -418,6 +442,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -431,6 +456,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -444,6 +470,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -457,6 +484,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -470,6 +498,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -483,6 +512,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -496,6 +526,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -509,6 +540,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -522,6 +554,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -535,6 +568,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -548,6 +582,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -561,6 +596,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -574,6 +610,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -587,6 +624,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -600,6 +638,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -613,6 +652,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -626,6 +666,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -639,6 +680,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -736,6 +778,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>S</t>
     </r>
@@ -749,6 +792,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -762,6 +806,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -775,6 +820,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -788,6 +834,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -801,6 +848,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -814,6 +862,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -824,6 +873,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -837,6 +887,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -847,6 +898,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -860,6 +912,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -870,6 +923,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -883,6 +937,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -893,6 +948,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M/L</t>
     </r>
@@ -906,6 +962,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>S</t>
     </r>
@@ -919,6 +976,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -932,6 +990,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -945,6 +1004,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -958,6 +1018,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -971,6 +1032,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -984,6 +1046,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -997,6 +1060,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1010,6 +1074,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1023,6 +1088,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1036,6 +1102,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1049,6 +1116,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1059,6 +1127,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1075,6 +1144,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>S</t>
     </r>
@@ -1085,6 +1155,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1098,6 +1169,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1111,6 +1183,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1124,6 +1197,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1134,6 +1208,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1144,6 +1219,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1154,6 +1230,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1167,6 +1244,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1177,6 +1255,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1187,6 +1266,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1197,6 +1277,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1210,6 +1291,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1220,6 +1302,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1230,6 +1313,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1240,6 +1324,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1253,6 +1338,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1266,6 +1352,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1276,6 +1363,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1289,6 +1377,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1302,6 +1391,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1315,6 +1405,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>S</t>
     </r>
@@ -1328,6 +1419,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>S</t>
     </r>
@@ -1341,6 +1433,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1351,6 +1444,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1361,6 +1455,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1371,6 +1466,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1384,6 +1480,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1397,6 +1494,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1407,6 +1505,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1417,6 +1516,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1427,6 +1527,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1440,6 +1541,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1453,6 +1555,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1463,6 +1566,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1473,6 +1577,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1483,6 +1588,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1496,6 +1602,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1506,6 +1613,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1516,6 +1624,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1526,6 +1635,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1539,6 +1649,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1549,6 +1660,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1559,6 +1671,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1569,6 +1682,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1582,6 +1696,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1592,6 +1707,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1602,6 +1718,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1612,6 +1729,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1625,6 +1743,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1635,6 +1754,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1645,6 +1765,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1655,6 +1776,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1668,6 +1790,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1678,6 +1801,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1688,6 +1812,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1701,6 +1826,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1711,6 +1837,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1721,6 +1848,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1731,6 +1859,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1744,6 +1873,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1754,6 +1884,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1764,6 +1895,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1774,6 +1906,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1787,6 +1920,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1800,6 +1934,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1813,6 +1948,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1823,6 +1959,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1833,6 +1970,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1843,6 +1981,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1856,6 +1995,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1869,6 +2009,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1879,6 +2020,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1889,6 +2031,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1899,6 +2042,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1912,6 +2056,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1925,6 +2070,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1938,6 +2084,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1948,6 +2095,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -1958,6 +2106,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -1968,6 +2117,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -1981,6 +2131,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -1991,6 +2142,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2001,6 +2153,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>XL</t>
     </r>
@@ -2011,6 +2164,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>JUMBO</t>
     </r>
@@ -2024,6 +2178,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>S</t>
     </r>
@@ -2334,6 +2489,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>MOONLIGHT</t>
     </r>
@@ -2344,6 +2500,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2354,6 +2511,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>OPALINE</t>
     </r>
@@ -2364,6 +2522,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2374,6 +2533,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>PARADISE</t>
     </r>
@@ -2384,6 +2544,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2394,6 +2555,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>PEARL</t>
     </r>
@@ -2404,6 +2566,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2414,6 +2577,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>PEARL</t>
     </r>
@@ -2424,6 +2588,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2434,6 +2599,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>SNAKESKIN</t>
     </r>
@@ -2444,6 +2610,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2454,6 +2621,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>SPARKING GOURAMI</t>
     </r>
@@ -2464,6 +2632,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2474,6 +2643,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>SUNSET  THICK LIPS</t>
     </r>
@@ -2484,6 +2654,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2494,6 +2665,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2510,6 +2682,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2523,6 +2696,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2536,6 +2710,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2549,6 +2724,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2562,6 +2738,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2575,6 +2752,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -2732,6 +2910,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>GARDNERI KILLIFISH</t>
     </r>
@@ -2742,6 +2921,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>M</t>
     </r>
@@ -2752,6 +2932,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>GOLDEN PANCHAX KILLIFISH</t>
     </r>
@@ -2762,6 +2943,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>L</t>
     </r>
@@ -3431,56 +3613,66 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -3802,7 +3994,7 @@
   <dimension ref="A1:E1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15694,19 +15886,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>